<commit_message>
working on adding image functionality
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -936,6 +936,66 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3838575" cy="3295650"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3838575" cy="3295650"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4170,6 +4230,7 @@
     <mergeCell ref="F53:G53"/>
   </mergeCells>
   <pageMargins left="0.47" right="0.36" top="0.47" bottom="0.21" header="0.2" footer="0.21"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6843,5 +6904,6 @@
     <mergeCell ref="F53:G53"/>
   </mergeCells>
   <pageMargins left="0.47" right="0.36" top="0.47" bottom="0.21" header="0.2" footer="0.21"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>